<commit_message>
Added basic conversion code
Supports fields except class and item, and the resulting spreadsheet is not formatted properly. Also, the example given for more than one item has the DD/MM/YYYY date format, but the previous example has the MM/DD/YYYY format, so I'm not sure about that.
</commit_message>
<xml_diff>
--- a/Sales Receipts.xlsx
+++ b/Sales Receipts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Customer</t>
   </si>
@@ -57,13 +57,51 @@
   </si>
   <si>
     <t>Template Name</t>
+  </si>
+  <si>
+    <t>PRODUCTS</t>
+  </si>
+  <si>
+    <t>Customer One</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>19.99</t>
+  </si>
+  <si>
+    <t>Customer Sales Receipt</t>
+  </si>
+  <si>
+    <t>29.99</t>
+  </si>
+  <si>
+    <t>14.99</t>
+  </si>
+  <si>
+    <t>Customer Two</t>
+  </si>
+  <si>
+    <t>3.99</t>
+  </si>
+  <si>
+    <t>4.99</t>
+  </si>
+  <si>
+    <t>16/01/2019</t>
+  </si>
+  <si>
+    <t>Customer Three</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -93,8 +131,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -392,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +483,240 @@
         <v>13</v>
       </c>
     </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s"/>
+      <c r="F2" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G2" t="s"/>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s"/>
+      <c r="F3" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G3" t="s"/>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s"/>
+      <c r="F4" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G4" t="s"/>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s"/>
+      <c r="F5" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G5" t="s"/>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="n">
+        <v>94.95</v>
+      </c>
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s"/>
+      <c r="F6" t="n">
+        <v>4789</v>
+      </c>
+      <c r="G6" t="s"/>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s"/>
+      <c r="F7" t="n">
+        <v>4789</v>
+      </c>
+      <c r="G7" t="s"/>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s"/>
+      <c r="F8" t="n">
+        <v>4789</v>
+      </c>
+      <c r="G8" t="s"/>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="n">
+        <v>30.96</v>
+      </c>
+      <c r="N8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s"/>
+      <c r="F9" t="n">
+        <v>5568</v>
+      </c>
+      <c r="G9" t="s"/>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s"/>
+      <c r="F10" t="n">
+        <v>5568</v>
+      </c>
+      <c r="G10" t="s"/>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="n">
+        <v>22.97</v>
+      </c>
+      <c r="N10" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "some cells written"
This reverts commit 37af9124c52f6b06c88fee5f1dd87ec6a3f09a5a.
</commit_message>
<xml_diff>
--- a/Sales Receipts.xlsx
+++ b/Sales Receipts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Customer</t>
   </si>
@@ -57,30 +57,13 @@
   </si>
   <si>
     <t>Template Name</t>
-  </si>
-  <si>
-    <t>PRODUCTS</t>
-  </si>
-  <si>
-    <t>Cyrus Goodman</t>
-  </si>
-  <si>
-    <t>Authorize.net</t>
-  </si>
-  <si>
-    <t>Custom Sales Receipt</t>
-  </si>
-  <si>
-    <t>Andi Mac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -110,9 +93,8 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -410,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,46 +444,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>43467</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5046</v>
-      </c>
-      <c r="N2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>43467</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="n">
-        <v>5054</v>
-      </c>
-      <c r="N3" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Separated orders by class and added shipping costs
</commit_message>
<xml_diff>
--- a/Sales Receipts.xlsx
+++ b/Sales Receipts.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sales Receipts" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sales Receipts" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>Customer</t>
   </si>
@@ -74,24 +74,18 @@
     <t>MED MENU BOOK</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>14.99</t>
-  </si>
-  <si>
     <t>Customer Sales Receipt</t>
   </si>
   <si>
+    <t>POSTAGE &amp; DEL</t>
+  </si>
+  <si>
     <t>Two Two</t>
   </si>
   <si>
     <t>MED MENU EBOOK</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Three Three</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>MED BUNDLE</t>
   </si>
   <si>
-    <t>19.99</t>
-  </si>
-  <si>
     <t>Five Five</t>
   </si>
   <si>
@@ -122,7 +113,7 @@
     <t>Ten Ten</t>
   </si>
   <si>
-    <t>Eleven Eleven</t>
+    <t>Eleven Eleven1</t>
   </si>
   <si>
     <t>027 OVN - VEG</t>
@@ -131,6 +122,9 @@
     <t>VEG MENU</t>
   </si>
   <si>
+    <t>Eleven Eleven2</t>
+  </si>
+  <si>
     <t>Whole Grains:035 WGC</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>PYRAMID - SM</t>
   </si>
   <si>
-    <t>3.99</t>
-  </si>
-  <si>
     <t>13/01/2019</t>
   </si>
   <si>
@@ -158,13 +149,13 @@
     <t>Fifteen Fifteen</t>
   </si>
   <si>
-    <t>Sixteen Sixteen</t>
+    <t>Sixteen Sixteen1</t>
   </si>
   <si>
     <t>MED GROCERY PAD</t>
   </si>
   <si>
-    <t>7.99</t>
+    <t>Sixteen Sixteen2</t>
   </si>
   <si>
     <t>VEG 12 WAYS BOOK</t>
@@ -185,31 +176,31 @@
     <t>MED MAGNET</t>
   </si>
   <si>
-    <t>4.99</t>
-  </si>
-  <si>
-    <t>Customer One</t>
+    <t>Customer One1</t>
+  </si>
+  <si>
+    <t>003 AHH</t>
+  </si>
+  <si>
+    <t>AH Brochure</t>
+  </si>
+  <si>
+    <t>AH Poster</t>
+  </si>
+  <si>
+    <t>Customer One2</t>
+  </si>
+  <si>
+    <t>VEG 12 WAYS EBOOK</t>
+  </si>
+  <si>
+    <t>Customer One3</t>
   </si>
   <si>
     <t>050 MISC:050-1 MISC</t>
   </si>
   <si>
     <t>LATIN POSTER</t>
-  </si>
-  <si>
-    <t>003 AHH</t>
-  </si>
-  <si>
-    <t>AH Brochure</t>
-  </si>
-  <si>
-    <t>29.99</t>
-  </si>
-  <si>
-    <t>AH Poster</t>
-  </si>
-  <si>
-    <t>VEG 12 WAYS EBOOK</t>
   </si>
   <si>
     <t>Customer Two</t>
@@ -557,7 +548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,17 +622,14 @@
       <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="n">
-        <v>36.97</v>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="n">
+        <v>14.99</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -652,7 +640,7 @@
         <v>43770</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -661,22 +649,22 @@
         <v>17</v>
       </c>
       <c r="F3" t="n">
-        <v>5506</v>
+        <v>5505</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
         <v>20</v>
       </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>6.99</v>
+      </c>
       <c r="K3" t="n">
-        <v>14.99</v>
+        <v>36.97</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -687,7 +675,7 @@
         <v>43770</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -696,22 +684,22 @@
         <v>17</v>
       </c>
       <c r="F4" t="n">
-        <v>5507</v>
+        <v>5506</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>14.99</v>
       </c>
       <c r="K4" t="n">
         <v>14.99</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -722,7 +710,7 @@
         <v>43770</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -731,22 +719,22 @@
         <v>17</v>
       </c>
       <c r="F5" t="n">
-        <v>5508</v>
+        <v>5507</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>14.99</v>
       </c>
       <c r="K5" t="n">
-        <v>23.98</v>
+        <v>14.99</v>
       </c>
       <c r="N5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -757,7 +745,7 @@
         <v>43770</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -766,22 +754,19 @@
         <v>17</v>
       </c>
       <c r="F6" t="n">
-        <v>5509</v>
+        <v>5508</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" t="n">
-        <v>18.98</v>
+        <v>25</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>19.99</v>
       </c>
       <c r="N6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -792,7 +777,7 @@
         <v>43770</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -801,22 +786,22 @@
         <v>17</v>
       </c>
       <c r="F7" t="n">
-        <v>5511</v>
+        <v>5508</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" t="s">
         <v>20</v>
       </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>3.99</v>
+      </c>
       <c r="K7" t="n">
-        <v>14.99</v>
+        <v>23.98</v>
       </c>
       <c r="N7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -824,10 +809,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>43800</v>
+        <v>43770</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -836,22 +821,19 @@
         <v>17</v>
       </c>
       <c r="F8" t="n">
-        <v>5512</v>
+        <v>5509</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" t="n">
-        <v>36.97</v>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>14.99</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -859,10 +841,10 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>43800</v>
+        <v>43770</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -871,22 +853,22 @@
         <v>17</v>
       </c>
       <c r="F9" t="n">
-        <v>5513</v>
+        <v>5509</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" t="s">
         <v>20</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3.99</v>
       </c>
       <c r="K9" t="n">
         <v>18.98</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -894,10 +876,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>43800</v>
+        <v>43770</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -906,22 +888,22 @@
         <v>17</v>
       </c>
       <c r="F10" t="n">
-        <v>5515</v>
+        <v>5511</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>14.99</v>
       </c>
       <c r="K10" t="n">
         <v>14.99</v>
       </c>
       <c r="N10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -932,7 +914,7 @@
         <v>43800</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -941,22 +923,19 @@
         <v>17</v>
       </c>
       <c r="F11" t="n">
-        <v>5516</v>
+        <v>5512</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" t="n">
+        <v>18</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="n">
         <v>14.99</v>
       </c>
       <c r="N11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -967,28 +946,31 @@
         <v>43800</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
       <c r="F12" t="n">
-        <v>5517</v>
+        <v>5512</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" t="s">
         <v>20</v>
       </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="K12" t="n">
+        <v>36.97</v>
+      </c>
       <c r="N12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -999,31 +981,28 @@
         <v>43800</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
       <c r="F13" t="n">
-        <v>5517</v>
+        <v>5513</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" t="n">
-        <v>36.97</v>
+        <v>18</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>14.99</v>
       </c>
       <c r="N13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1034,7 +1013,7 @@
         <v>43800</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1043,22 +1022,22 @@
         <v>17</v>
       </c>
       <c r="F14" t="n">
-        <v>5518</v>
+        <v>5513</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" t="s">
         <v>20</v>
       </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>3.99</v>
+      </c>
       <c r="K14" t="n">
-        <v>14.99</v>
+        <v>18.98</v>
       </c>
       <c r="N14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1069,7 +1048,7 @@
         <v>43800</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
@@ -1078,33 +1057,33 @@
         <v>17</v>
       </c>
       <c r="F15" t="n">
-        <v>5519</v>
+        <v>5515</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>14.99</v>
       </c>
       <c r="K15" t="n">
-        <v>7.98</v>
+        <v>14.99</v>
       </c>
       <c r="N15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>44</v>
+      <c r="B16" s="1" t="n">
+        <v>43800</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -1113,132 +1092,132 @@
         <v>17</v>
       </c>
       <c r="F16" t="n">
-        <v>5521</v>
+        <v>5516</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>14.99</v>
       </c>
       <c r="K16" t="n">
-        <v>18.98</v>
+        <v>14.99</v>
       </c>
       <c r="N16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>44</v>
+      <c r="B17" s="1" t="n">
+        <v>43800</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
         <v>17</v>
       </c>
       <c r="F17" t="n">
-        <v>5523</v>
+        <v>5517</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" t="n">
+        <v>34</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
         <v>14.99</v>
       </c>
       <c r="N17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
-        <v>44</v>
+      <c r="B18" s="1" t="n">
+        <v>43800</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
       </c>
       <c r="F18" t="n">
-        <v>5525</v>
+        <v>5517</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J18" t="n">
+        <v>18.49</v>
       </c>
       <c r="N18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>44</v>
+      <c r="B19" s="1" t="n">
+        <v>43800</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
       </c>
       <c r="F19" t="n">
-        <v>5525</v>
+        <v>5517</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" t="s">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>14.99</v>
       </c>
       <c r="N19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
-        <v>44</v>
+      <c r="B20" s="1" t="n">
+        <v>43800</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
@@ -1247,33 +1226,36 @@
         <v>17</v>
       </c>
       <c r="F20" t="n">
-        <v>5525</v>
+        <v>5517</v>
       </c>
       <c r="G20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" t="s">
         <v>20</v>
       </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="J20" t="n">
+        <v>18.48</v>
+      </c>
       <c r="K20" t="n">
-        <v>44.96</v>
+        <v>36.97</v>
       </c>
       <c r="N20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
-        <v>44</v>
+      <c r="B21" s="1" t="n">
+        <v>43800</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
         <v>16</v>
@@ -1282,33 +1264,33 @@
         <v>17</v>
       </c>
       <c r="F21" t="n">
-        <v>5526</v>
+        <v>5518</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>14.99</v>
       </c>
       <c r="K21" t="n">
-        <v>18.98</v>
+        <v>14.99</v>
       </c>
       <c r="N21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>14</v>
       </c>
-      <c r="B22" t="s">
-        <v>44</v>
+      <c r="B22" s="1" t="n">
+        <v>43800</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
@@ -1317,33 +1299,30 @@
         <v>17</v>
       </c>
       <c r="F22" t="n">
-        <v>5527</v>
+        <v>5519</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" t="n">
-        <v>18.98</v>
+        <v>40</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3.99</v>
       </c>
       <c r="N22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B23" t="s">
-        <v>44</v>
+      <c r="B23" s="1" t="n">
+        <v>43800</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
         <v>16</v>
@@ -1352,22 +1331,22 @@
         <v>17</v>
       </c>
       <c r="F23" t="n">
-        <v>5528</v>
+        <v>5519</v>
       </c>
       <c r="G23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" t="s">
         <v>20</v>
       </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>3.99</v>
+      </c>
       <c r="K23" t="n">
-        <v>14.99</v>
+        <v>7.98</v>
       </c>
       <c r="N23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1375,10 +1354,10 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
@@ -1387,19 +1366,19 @@
         <v>17</v>
       </c>
       <c r="F24" t="n">
-        <v>5530</v>
+        <v>5521</v>
       </c>
       <c r="G24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H24" t="s">
-        <v>24</v>
-      </c>
-      <c r="I24" t="s">
-        <v>43</v>
+        <v>18</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>14.99</v>
       </c>
       <c r="N24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1407,10 +1386,10 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
         <v>16</v>
@@ -1419,19 +1398,22 @@
         <v>17</v>
       </c>
       <c r="F25" t="n">
-        <v>5530</v>
+        <v>5521</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" t="s">
-        <v>56</v>
+        <v>20</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="K25" t="n">
+        <v>18.98</v>
       </c>
       <c r="N25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1439,10 +1421,10 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
@@ -1451,196 +1433,202 @@
         <v>17</v>
       </c>
       <c r="F26" t="n">
-        <v>5530</v>
+        <v>5523</v>
       </c>
       <c r="G26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H26" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>14.99</v>
       </c>
       <c r="K26" t="n">
-        <v>35.96</v>
+        <v>14.99</v>
       </c>
       <c r="N26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="1" t="n">
-        <v>43230</v>
+      <c r="B27" t="s">
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="E27" t="s">
         <v>17</v>
       </c>
       <c r="F27" t="n">
-        <v>4787</v>
+        <v>5525</v>
       </c>
       <c r="G27" t="s">
-        <v>59</v>
-      </c>
-      <c r="H27" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27" t="s">
-        <v>28</v>
+        <v>45</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>7.99</v>
       </c>
       <c r="N27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="1" t="n">
-        <v>43230</v>
+      <c r="B28" t="s">
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
         <v>17</v>
       </c>
       <c r="F28" t="n">
-        <v>4787</v>
+        <v>5525</v>
       </c>
       <c r="G28" t="s">
-        <v>61</v>
-      </c>
-      <c r="H28" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28" t="s">
-        <v>62</v>
+        <v>18</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>14.99</v>
       </c>
       <c r="N28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="1" t="n">
-        <v>43230</v>
+      <c r="B29" t="s">
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="E29" t="s">
         <v>17</v>
       </c>
       <c r="F29" t="n">
-        <v>4787</v>
+        <v>5525</v>
       </c>
       <c r="G29" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J29" t="n">
+        <v>26.48</v>
       </c>
       <c r="N29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="1" t="n">
-        <v>43230</v>
+      <c r="B30" t="s">
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
       </c>
       <c r="F30" t="n">
-        <v>4787</v>
+        <v>5525</v>
       </c>
       <c r="G30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" t="s">
-        <v>20</v>
-      </c>
-      <c r="K30" t="n">
-        <v>94.95</v>
+        <v>47</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>14.99</v>
       </c>
       <c r="N30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="1" t="n">
-        <v>43230</v>
+      <c r="B31" t="s">
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E31" t="s">
         <v>17</v>
       </c>
       <c r="F31" t="n">
-        <v>4789</v>
+        <v>5525</v>
       </c>
       <c r="G31" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" t="s">
-        <v>43</v>
+        <v>20</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="J31" t="n">
+        <v>18.48</v>
+      </c>
+      <c r="K31" t="n">
+        <v>44.96</v>
       </c>
       <c r="N31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="1" t="n">
-        <v>43230</v>
+      <c r="B32" t="s">
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D32" t="s">
         <v>16</v>
@@ -1649,30 +1637,30 @@
         <v>17</v>
       </c>
       <c r="F32" t="n">
-        <v>4789</v>
+        <v>5526</v>
       </c>
       <c r="G32" t="s">
-        <v>55</v>
-      </c>
-      <c r="H32" t="s">
-        <v>24</v>
-      </c>
-      <c r="I32" t="s">
-        <v>56</v>
+        <v>18</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>14.99</v>
       </c>
       <c r="N32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="1" t="n">
-        <v>43230</v>
+      <c r="B33" t="s">
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D33" t="s">
         <v>16</v>
@@ -1681,22 +1669,22 @@
         <v>17</v>
       </c>
       <c r="F33" t="n">
-        <v>4789</v>
+        <v>5526</v>
       </c>
       <c r="G33" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" t="s">
-        <v>24</v>
-      </c>
-      <c r="I33" t="s">
         <v>20</v>
       </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>3.99</v>
+      </c>
       <c r="K33" t="n">
-        <v>30.96</v>
+        <v>18.98</v>
       </c>
       <c r="N33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -1704,10 +1692,10 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
         <v>16</v>
@@ -1716,19 +1704,19 @@
         <v>17</v>
       </c>
       <c r="F34" t="n">
-        <v>5568</v>
+        <v>5527</v>
       </c>
       <c r="G34" t="s">
-        <v>42</v>
-      </c>
-      <c r="H34" t="s">
-        <v>24</v>
-      </c>
-      <c r="I34" t="s">
-        <v>43</v>
+        <v>18</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>14.99</v>
       </c>
       <c r="N34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -1736,10 +1724,10 @@
         <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
         <v>16</v>
@@ -1748,22 +1736,654 @@
         <v>17</v>
       </c>
       <c r="F35" t="n">
+        <v>5527</v>
+      </c>
+      <c r="G35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="K35" t="n">
+        <v>18.98</v>
+      </c>
+      <c r="N35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" t="n">
+        <v>5528</v>
+      </c>
+      <c r="G36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="K36" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="N36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" t="n">
+        <v>5530</v>
+      </c>
+      <c r="G37" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="N37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" t="n">
+        <v>5530</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="N38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" t="n">
+        <v>5530</v>
+      </c>
+      <c r="G39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="N39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" t="n">
+        <v>5530</v>
+      </c>
+      <c r="G40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="K40" t="n">
+        <v>35.96</v>
+      </c>
+      <c r="N40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G41" t="s">
+        <v>55</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="N41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G42" t="s">
+        <v>56</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="N42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G43" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="J43" t="n">
+        <v>53.31</v>
+      </c>
+      <c r="N43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G44" t="s">
+        <v>58</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="N44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G45" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="J45" t="n">
+        <v>18.32</v>
+      </c>
+      <c r="N45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G46" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="N46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" t="n">
+        <v>4787</v>
+      </c>
+      <c r="G47" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I47" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="J47" t="n">
+        <v>23.32</v>
+      </c>
+      <c r="K47" t="n">
+        <v>94.95</v>
+      </c>
+      <c r="N47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C48" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" t="n">
+        <v>4789</v>
+      </c>
+      <c r="G48" t="s">
+        <v>40</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1</v>
+      </c>
+      <c r="I48" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="N48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" t="n">
+        <v>4789</v>
+      </c>
+      <c r="G49" t="s">
+        <v>52</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="N49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C50" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" t="n">
+        <v>4789</v>
+      </c>
+      <c r="G50" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="N50" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>43230</v>
+      </c>
+      <c r="C51" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" t="n">
+        <v>4789</v>
+      </c>
+      <c r="G51" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1</v>
+      </c>
+      <c r="I51" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="K51" t="n">
+        <v>30.96</v>
+      </c>
+      <c r="N51" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" t="n">
         <v>5568</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G52" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="N52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" t="n">
+        <v>5568</v>
+      </c>
+      <c r="G53" t="s">
         <v>18</v>
       </c>
-      <c r="H35" t="s">
-        <v>24</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="H53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="N53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" t="n">
+        <v>5568</v>
+      </c>
+      <c r="G54" t="s">
         <v>20</v>
       </c>
-      <c r="K35" t="n">
+      <c r="H54" t="n">
+        <v>1</v>
+      </c>
+      <c r="I54" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="K54" t="n">
         <v>22.97</v>
       </c>
-      <c r="N35" t="s">
-        <v>21</v>
+      <c r="N54" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed csv to xlsx
</commit_message>
<xml_diff>
--- a/Sales Receipts.xlsx
+++ b/Sales Receipts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
   <si>
     <t>Customer</t>
   </si>
@@ -74,69 +74,96 @@
     <t>Authorize.net</t>
   </si>
   <si>
+    <t>5505</t>
+  </si>
+  <si>
     <t>MED MENU BOOK</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>14.99</t>
-  </si>
-  <si>
     <t>Customer Sales Receipt</t>
   </si>
   <si>
+    <t>POSTAGE &amp; DEL</t>
+  </si>
+  <si>
     <t>Two Two</t>
   </si>
   <si>
+    <t>5506</t>
+  </si>
+  <si>
     <t>MED MENU EBOOK</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Three Three</t>
   </si>
   <si>
+    <t>5507</t>
+  </si>
+  <si>
     <t>Four Four</t>
   </si>
   <si>
+    <t>5508</t>
+  </si>
+  <si>
     <t>MED BUNDLE</t>
   </si>
   <si>
-    <t>19.99</t>
-  </si>
-  <si>
     <t>Five Five</t>
   </si>
   <si>
+    <t>5509</t>
+  </si>
+  <si>
     <t>Six Six</t>
   </si>
   <si>
+    <t>5511</t>
+  </si>
+  <si>
     <t>01/12/2019</t>
   </si>
   <si>
     <t>Seven Seven</t>
   </si>
   <si>
+    <t>5512</t>
+  </si>
+  <si>
     <t>Eight Eight</t>
   </si>
   <si>
+    <t>5513</t>
+  </si>
+  <si>
     <t>Nine Nine</t>
   </si>
   <si>
+    <t>5515</t>
+  </si>
+  <si>
     <t>Ten Ten</t>
   </si>
   <si>
-    <t>Eleven Eleven</t>
+    <t>5516</t>
+  </si>
+  <si>
+    <t>Eleven Eleven1</t>
   </si>
   <si>
     <t>027 OVN - VEG</t>
   </si>
   <si>
+    <t>5517</t>
+  </si>
+  <si>
     <t>VEG MENU</t>
   </si>
   <si>
+    <t>Eleven Eleven2</t>
+  </si>
+  <si>
     <t>Whole Grains:035 WGC</t>
   </si>
   <si>
@@ -146,31 +173,43 @@
     <t>Twelve Twelve</t>
   </si>
   <si>
+    <t>5518</t>
+  </si>
+  <si>
     <t>Thirteen Thirteen</t>
   </si>
   <si>
+    <t>5519</t>
+  </si>
+  <si>
     <t>PYRAMID - SM</t>
   </si>
   <si>
-    <t>3.99</t>
-  </si>
-  <si>
     <t>01/13/2019</t>
   </si>
   <si>
     <t>Fourteen Fourteen</t>
   </si>
   <si>
+    <t>5521</t>
+  </si>
+  <si>
     <t>Fifteen Fifteen</t>
   </si>
   <si>
-    <t>Sixteen Sixteen</t>
+    <t>5523</t>
+  </si>
+  <si>
+    <t>Sixteen Sixteen1</t>
+  </si>
+  <si>
+    <t>5525</t>
   </si>
   <si>
     <t>MED GROCERY PAD</t>
   </si>
   <si>
-    <t>7.99</t>
+    <t>Sixteen Sixteen2</t>
   </si>
   <si>
     <t>VEG 12 WAYS BOOK</t>
@@ -179,25 +218,55 @@
     <t>Seventeen Seventeen</t>
   </si>
   <si>
+    <t>5526</t>
+  </si>
+  <si>
     <t>Eighteen Eighteen</t>
   </si>
   <si>
+    <t>5527</t>
+  </si>
+  <si>
     <t>Nineteen Nineteen</t>
   </si>
   <si>
+    <t>5528</t>
+  </si>
+  <si>
     <t>Twenty Twenty</t>
   </si>
   <si>
+    <t>5530</t>
+  </si>
+  <si>
     <t>MED MAGNET</t>
   </si>
   <si>
-    <t>4.99</t>
-  </si>
-  <si>
     <t>10/05/2018</t>
   </si>
   <si>
-    <t>Customer One</t>
+    <t>Customer One1</t>
+  </si>
+  <si>
+    <t>003 AHH</t>
+  </si>
+  <si>
+    <t>4787</t>
+  </si>
+  <si>
+    <t>AH Brochure</t>
+  </si>
+  <si>
+    <t>AH Poster</t>
+  </si>
+  <si>
+    <t>Customer One2</t>
+  </si>
+  <si>
+    <t>VEG 12 WAYS EBOOK</t>
+  </si>
+  <si>
+    <t>Customer One3</t>
   </si>
   <si>
     <t>050 MISC:050-1 MISC</t>
@@ -206,28 +275,19 @@
     <t>LATIN POSTER</t>
   </si>
   <si>
-    <t>003 AHH</t>
-  </si>
-  <si>
-    <t>AH Brochure</t>
-  </si>
-  <si>
-    <t>29.99</t>
-  </si>
-  <si>
-    <t>AH Poster</t>
-  </si>
-  <si>
-    <t>VEG 12 WAYS EBOOK</t>
-  </si>
-  <si>
     <t>Customer Two</t>
   </si>
   <si>
+    <t>4789</t>
+  </si>
+  <si>
     <t>01/16/2019</t>
   </si>
   <si>
     <t>Customer Three</t>
+  </si>
+  <si>
+    <t>5568</t>
   </si>
 </sst>
 </file>
@@ -563,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,23 +691,20 @@
       <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="n">
-        <v>5505</v>
+      <c r="F2" t="s">
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="n">
-        <v>36.97</v>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="n">
+        <v>14.99</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -658,7 +715,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -666,23 +723,23 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="n">
-        <v>5506</v>
+      <c r="F3" t="s">
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>6.99</v>
       </c>
       <c r="K3" t="n">
-        <v>14.99</v>
+        <v>36.97</v>
       </c>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -693,7 +750,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -701,23 +758,23 @@
       <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="n">
-        <v>5507</v>
+      <c r="F4" t="s">
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" t="s">
-        <v>21</v>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>14.99</v>
       </c>
       <c r="K4" t="n">
         <v>14.99</v>
       </c>
       <c r="N4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -728,31 +785,31 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="n">
-        <v>5508</v>
-      </c>
       <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" t="s">
         <v>25</v>
       </c>
-      <c r="I5" t="s">
-        <v>29</v>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>14.99</v>
       </c>
       <c r="K5" t="n">
-        <v>23.98</v>
+        <v>14.99</v>
       </c>
       <c r="N5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -763,31 +820,28 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="n">
-        <v>5509</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" t="n">
-        <v>18.98</v>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>19.99</v>
       </c>
       <c r="N6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -798,7 +852,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -806,23 +860,23 @@
       <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" t="n">
-        <v>5511</v>
+      <c r="F7" t="s">
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>3.99</v>
       </c>
       <c r="K7" t="n">
-        <v>14.99</v>
+        <v>23.98</v>
       </c>
       <c r="N7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -830,34 +884,31 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="n">
-        <v>5512</v>
-      </c>
       <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
         <v>20</v>
       </c>
-      <c r="I8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" t="n">
-        <v>36.97</v>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>14.99</v>
       </c>
       <c r="N8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -865,34 +916,34 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="n">
-        <v>5513</v>
-      </c>
       <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3.99</v>
       </c>
       <c r="K9" t="n">
         <v>18.98</v>
       </c>
       <c r="N9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -900,10 +951,10 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -911,23 +962,23 @@
       <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="F10" t="n">
-        <v>5515</v>
+      <c r="F10" t="s">
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" t="s">
         <v>25</v>
       </c>
-      <c r="I10" t="s">
-        <v>21</v>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>14.99</v>
       </c>
       <c r="K10" t="n">
         <v>14.99</v>
       </c>
       <c r="N10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -935,7 +986,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
@@ -946,23 +997,20 @@
       <c r="E11" t="s">
         <v>18</v>
       </c>
-      <c r="F11" t="n">
-        <v>5516</v>
+      <c r="F11" t="s">
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="n">
         <v>14.99</v>
       </c>
       <c r="N11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -970,31 +1018,34 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="n">
-        <v>5517</v>
-      </c>
       <c r="G12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="K12" t="n">
+        <v>36.97</v>
       </c>
       <c r="N12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1002,34 +1053,31 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" t="n">
-        <v>5517</v>
+      <c r="F13" t="s">
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" t="n">
-        <v>36.97</v>
+        <v>20</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>14.99</v>
       </c>
       <c r="N13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1037,10 +1085,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -1048,23 +1096,23 @@
       <c r="E14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" t="n">
-        <v>5518</v>
+      <c r="F14" t="s">
+        <v>39</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>3.99</v>
       </c>
       <c r="K14" t="n">
-        <v>14.99</v>
+        <v>18.98</v>
       </c>
       <c r="N14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1072,10 +1120,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1083,23 +1131,23 @@
       <c r="E15" t="s">
         <v>18</v>
       </c>
-      <c r="F15" t="n">
-        <v>5519</v>
+      <c r="F15" t="s">
+        <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" t="s">
         <v>25</v>
       </c>
-      <c r="I15" t="s">
-        <v>45</v>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>14.99</v>
       </c>
       <c r="K15" t="n">
-        <v>7.98</v>
+        <v>14.99</v>
       </c>
       <c r="N15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1107,10 +1155,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -1118,23 +1166,23 @@
       <c r="E16" t="s">
         <v>18</v>
       </c>
-      <c r="F16" t="n">
-        <v>5521</v>
+      <c r="F16" t="s">
+        <v>43</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" t="s">
         <v>25</v>
       </c>
-      <c r="I16" t="s">
-        <v>21</v>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>14.99</v>
       </c>
       <c r="K16" t="n">
-        <v>18.98</v>
+        <v>14.99</v>
       </c>
       <c r="N16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1142,34 +1190,31 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" t="n">
-        <v>5523</v>
-      </c>
       <c r="G17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" t="n">
+        <v>47</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
         <v>14.99</v>
       </c>
       <c r="N17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1177,31 +1222,34 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
         <v>46</v>
       </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" t="n">
-        <v>5525</v>
-      </c>
       <c r="G18" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" t="s">
-        <v>51</v>
+        <v>22</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J18" t="n">
+        <v>18.49</v>
       </c>
       <c r="N18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1209,31 +1257,31 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" t="n">
-        <v>5525</v>
-      </c>
       <c r="G19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>14.99</v>
       </c>
       <c r="N19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1241,34 +1289,37 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
         <v>46</v>
       </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" t="n">
-        <v>5525</v>
-      </c>
       <c r="G20" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="J20" t="n">
+        <v>18.48</v>
       </c>
       <c r="K20" t="n">
-        <v>44.96</v>
+        <v>36.97</v>
       </c>
       <c r="N20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1276,10 +1327,10 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
@@ -1287,23 +1338,23 @@
       <c r="E21" t="s">
         <v>18</v>
       </c>
-      <c r="F21" t="n">
-        <v>5526</v>
+      <c r="F21" t="s">
+        <v>52</v>
       </c>
       <c r="G21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" t="s">
         <v>25</v>
       </c>
-      <c r="I21" t="s">
-        <v>21</v>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>14.99</v>
       </c>
       <c r="K21" t="n">
-        <v>18.98</v>
+        <v>14.99</v>
       </c>
       <c r="N21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1311,34 +1362,31 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
         <v>54</v>
       </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" t="n">
-        <v>5527</v>
-      </c>
       <c r="G22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" t="n">
-        <v>18.98</v>
+        <v>55</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3.99</v>
       </c>
       <c r="N22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1346,10 +1394,10 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -1357,23 +1405,23 @@
       <c r="E23" t="s">
         <v>18</v>
       </c>
-      <c r="F23" t="n">
-        <v>5528</v>
+      <c r="F23" t="s">
+        <v>54</v>
       </c>
       <c r="G23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>3.99</v>
       </c>
       <c r="K23" t="n">
-        <v>14.99</v>
+        <v>7.98</v>
       </c>
       <c r="N23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1381,10 +1429,10 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -1392,20 +1440,20 @@
       <c r="E24" t="s">
         <v>18</v>
       </c>
-      <c r="F24" t="n">
-        <v>5530</v>
+      <c r="F24" t="s">
+        <v>58</v>
       </c>
       <c r="G24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" t="s">
-        <v>45</v>
+        <v>20</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>14.99</v>
       </c>
       <c r="N24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1413,10 +1461,10 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -1424,20 +1472,23 @@
       <c r="E25" t="s">
         <v>18</v>
       </c>
-      <c r="F25" t="n">
-        <v>5530</v>
+      <c r="F25" t="s">
+        <v>58</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
-      </c>
-      <c r="H25" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" t="s">
-        <v>58</v>
+        <v>22</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="K25" t="n">
+        <v>18.98</v>
       </c>
       <c r="N25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1445,10 +1496,10 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
@@ -1456,23 +1507,23 @@
       <c r="E26" t="s">
         <v>18</v>
       </c>
-      <c r="F26" t="n">
-        <v>5530</v>
+      <c r="F26" t="s">
+        <v>60</v>
       </c>
       <c r="G26" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" t="s">
         <v>25</v>
       </c>
-      <c r="I26" t="s">
-        <v>29</v>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>14.99</v>
       </c>
       <c r="K26" t="n">
-        <v>35.96</v>
+        <v>14.99</v>
       </c>
       <c r="N26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -1480,31 +1531,31 @@
         <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
       </c>
-      <c r="F27" t="n">
-        <v>4787</v>
+      <c r="F27" t="s">
+        <v>62</v>
       </c>
       <c r="G27" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" t="s">
-        <v>29</v>
+        <v>63</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>7.99</v>
       </c>
       <c r="N27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -1512,31 +1563,31 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
         <v>18</v>
       </c>
-      <c r="F28" t="n">
-        <v>4787</v>
+      <c r="F28" t="s">
+        <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" t="s">
-        <v>65</v>
+        <v>20</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>14.99</v>
       </c>
       <c r="N28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1544,31 +1595,34 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
         <v>18</v>
       </c>
-      <c r="F29" t="n">
-        <v>4787</v>
+      <c r="F29" t="s">
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>66</v>
-      </c>
-      <c r="H29" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J29" t="n">
+        <v>26.48</v>
       </c>
       <c r="N29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -1576,34 +1630,31 @@
         <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
         <v>18</v>
       </c>
-      <c r="F30" t="n">
-        <v>4787</v>
+      <c r="F30" t="s">
+        <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>67</v>
-      </c>
-      <c r="H30" t="s">
-        <v>25</v>
-      </c>
-      <c r="I30" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" t="n">
-        <v>94.95</v>
+        <v>65</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>14.99</v>
       </c>
       <c r="N30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -1611,31 +1662,37 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
         <v>18</v>
       </c>
-      <c r="F31" t="n">
-        <v>4789</v>
+      <c r="F31" t="s">
+        <v>62</v>
       </c>
       <c r="G31" t="s">
-        <v>44</v>
-      </c>
-      <c r="H31" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" t="s">
-        <v>45</v>
+        <v>22</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="J31" t="n">
+        <v>18.48</v>
+      </c>
+      <c r="K31" t="n">
+        <v>44.96</v>
       </c>
       <c r="N31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -1643,10 +1700,10 @@
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
@@ -1654,20 +1711,20 @@
       <c r="E32" t="s">
         <v>18</v>
       </c>
-      <c r="F32" t="n">
-        <v>4789</v>
+      <c r="F32" t="s">
+        <v>67</v>
       </c>
       <c r="G32" t="s">
-        <v>57</v>
-      </c>
-      <c r="H32" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" t="s">
-        <v>58</v>
+        <v>20</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>14.99</v>
       </c>
       <c r="N32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -1675,10 +1732,10 @@
         <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
@@ -1686,23 +1743,23 @@
       <c r="E33" t="s">
         <v>18</v>
       </c>
-      <c r="F33" t="n">
-        <v>4789</v>
+      <c r="F33" t="s">
+        <v>67</v>
       </c>
       <c r="G33" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" t="s">
-        <v>25</v>
-      </c>
-      <c r="I33" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>3.99</v>
       </c>
       <c r="K33" t="n">
-        <v>30.96</v>
+        <v>18.98</v>
       </c>
       <c r="N33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -1710,31 +1767,31 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
         <v>69</v>
       </c>
-      <c r="C34" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" t="n">
-        <v>5568</v>
-      </c>
       <c r="G34" t="s">
-        <v>44</v>
-      </c>
-      <c r="H34" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" t="s">
-        <v>45</v>
+        <v>20</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>14.99</v>
       </c>
       <c r="N34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -1742,34 +1799,666 @@
         <v>14</v>
       </c>
       <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" t="s">
         <v>69</v>
       </c>
-      <c r="C35" t="s">
+      <c r="G35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="K35" t="n">
+        <v>18.98</v>
+      </c>
+      <c r="N35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" t="s">
         <v>70</v>
       </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" t="n">
-        <v>5568</v>
-      </c>
-      <c r="G35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" t="s">
         <v>25</v>
       </c>
-      <c r="I35" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" t="n">
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="K36" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="N36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" t="s">
+        <v>55</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="N37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" t="s">
+        <v>74</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="N38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="N39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>73</v>
+      </c>
+      <c r="G40" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="K40" t="n">
+        <v>35.96</v>
+      </c>
+      <c r="N40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
+        <v>78</v>
+      </c>
+      <c r="G41" t="s">
+        <v>79</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="N41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" t="s">
+        <v>78</v>
+      </c>
+      <c r="G42" t="s">
+        <v>80</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="N42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" t="s">
+        <v>78</v>
+      </c>
+      <c r="G43" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="J43" t="n">
+        <v>53.31</v>
+      </c>
+      <c r="N43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" t="s">
+        <v>78</v>
+      </c>
+      <c r="G44" t="s">
+        <v>82</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="N44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="J45" t="n">
+        <v>18.32</v>
+      </c>
+      <c r="N45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" t="s">
+        <v>78</v>
+      </c>
+      <c r="G46" t="s">
+        <v>85</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="N46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" t="s">
+        <v>83</v>
+      </c>
+      <c r="D47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I47" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="J47" t="n">
+        <v>23.32</v>
+      </c>
+      <c r="K47" t="n">
+        <v>94.95</v>
+      </c>
+      <c r="N47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" t="s">
+        <v>87</v>
+      </c>
+      <c r="G48" t="s">
+        <v>55</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1</v>
+      </c>
+      <c r="I48" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="N48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" t="s">
+        <v>87</v>
+      </c>
+      <c r="G49" t="s">
+        <v>74</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="N49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" t="s">
+        <v>87</v>
+      </c>
+      <c r="G50" t="s">
+        <v>20</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="N50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" t="s">
+        <v>87</v>
+      </c>
+      <c r="G51" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1</v>
+      </c>
+      <c r="I51" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="K51" t="n">
+        <v>30.96</v>
+      </c>
+      <c r="N51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" t="s">
+        <v>90</v>
+      </c>
+      <c r="G52" t="s">
+        <v>55</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="N52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" t="s">
+        <v>89</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" t="s">
+        <v>90</v>
+      </c>
+      <c r="G53" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="N53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" t="s">
+        <v>90</v>
+      </c>
+      <c r="G54" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" t="n">
+        <v>1</v>
+      </c>
+      <c r="I54" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="K54" t="n">
         <v>22.97</v>
       </c>
-      <c r="N35" t="s">
-        <v>22</v>
+      <c r="N54" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>